<commit_message>
Added vapor pressure deficit to aggregations
- New function ‘vp0’ to calculate saturation vapor pressure
- New function ‘vpd’ to calculate vapor pressure deficit
- Updated aggregation ‘dailyThermalDrynessStress’ from using maximum
daily temperature to VPD based on minimum and maximum daily temperature
and mean monthly relative humidity
- Added aggregation ‘monthlyVPD’
- Updated code part 1 of test project to reflect changes
- Updated excel spreadsheet that explains overall aggregation output


Former-commit-id: ca78659ece0a3a6b5875ba1ec00b40fd20747ee9 [formerly 74bb3242b50cb39c4242ca3b1b8df4047f6cf11e]
Former-commit-id: 4fef25ec234989d11e454cfd0ab7219ed8f47b00
</commit_message>
<xml_diff>
--- a/Database_Stuff/Explanation_output_variables_overall_aggregation.xlsx
+++ b/Database_Stuff/Explanation_output_variables_overall_aggregation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-36040" yWindow="0" windowWidth="32400" windowHeight="19580" tabRatio="1000"/>
+    <workbookView xWindow="-40880" yWindow="0" windowWidth="39560" windowHeight="20920" tabRatio="1000"/>
   </bookViews>
   <sheets>
     <sheet name="aggregation_overall" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4398" uniqueCount="1797">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4466" uniqueCount="1830">
   <si>
     <t>P_id</t>
   </si>
@@ -5389,28 +5389,127 @@
     <t>End DOY of longest continuous topsoil dry period (&lt; X MPa) when air Tmean &gt; 0 C</t>
   </si>
   <si>
-    <t>Mean10HottestDays_AirTmax_mean</t>
-  </si>
-  <si>
-    <t>Mean10HottestDays_AirTmax_MoistureStress_SWPcritXkPa_allLayers_mean</t>
-  </si>
-  <si>
-    <t>Mean10HottestDays_AirTmax_MoistureStress_SWPcritXkPa_topLayer_mean</t>
-  </si>
-  <si>
-    <t>Mean10HottestDays_AirTmax_MoistureStress_SWPcritXkPa_bottomLayer_mean</t>
-  </si>
-  <si>
-    <t>Mean10HottestDays_AirTmax_max</t>
-  </si>
-  <si>
-    <t>Mean10HottestDays_AirTmax_MoistureStress_SWPcritXkPa_allLayers_max</t>
-  </si>
-  <si>
-    <t>Mean10HottestDays_AirTmax_MoistureStress_SWPcritXkPa_topLayer_max</t>
-  </si>
-  <si>
-    <t>Mean10HottestDays_AirTmax_MoistureStress_SWPcritXkPa_bottomLayer_max</t>
+    <t>Mean10HottestDays_VPD_kPa_mean</t>
+  </si>
+  <si>
+    <t>Mean10HottestDays_VPD_kPa_MoistureStress_SWPcritXkPa_allLayers_mean</t>
+  </si>
+  <si>
+    <t>Mean10HottestDays_VPD_kPa_MoistureStress_SWPcritXkPa_topLayer_mean</t>
+  </si>
+  <si>
+    <t>Mean10HottestDays_VPD_kPa_MoistureStress_SWPcritXkPa_bottomLayer_mean</t>
+  </si>
+  <si>
+    <t>Mean10HottestDays_VPD_kPa_max</t>
+  </si>
+  <si>
+    <t>Mean10HottestDays_VPD_kPa_MoistureStress_SWPcritXkPa_allLayers_max</t>
+  </si>
+  <si>
+    <t>Mean10HottestDays_VPD_kPa_MoistureStress_SWPcritXkPa_topLayer_max</t>
+  </si>
+  <si>
+    <t>Mean10HottestDays_VPD_kPa_MoistureStress_SWPcritXkPa_bottomLayer_max</t>
+  </si>
+  <si>
+    <t>Mean across years of mean vapur pressure deficit (kPa) of the 10 hottest days per year</t>
+  </si>
+  <si>
+    <t>Mean across years of mean vapur pressure deficit (kPa) of the 10 hottest days per year when SWP in each soil layer &lt; X MPa</t>
+  </si>
+  <si>
+    <t>Mean across years of mean vapur pressure deficit (kPa) of the 10 hottest days per year when SWP in each top soil layer &lt; X MPa</t>
+  </si>
+  <si>
+    <t>Mean across years of mean vapur pressure deficit (kPa) of the 10 hottest days per year when SWP in each bottom soil layer &lt; X MPa</t>
+  </si>
+  <si>
+    <t>Maximum across years of mean vapur pressure deficit (kPa) of the 10 hottest days per year when SWP in each soil layer &lt; X MPa</t>
+  </si>
+  <si>
+    <t>Maximum across years of mean vapur pressure deficit (kPa) of the 10 hottest days per year when SWP in each top soil layer &lt; X MPa</t>
+  </si>
+  <si>
+    <t>Maximum across years of mean vapur pressure deficit (kPa) of the 10 hottest days per year when SWP in each bottom soil layer &lt; X MPa</t>
+  </si>
+  <si>
+    <t>Maximum across years of mean vapur pressure deficit (kPa) of the 10 hottest days per year</t>
+  </si>
+  <si>
+    <t>monthlyVPD</t>
+  </si>
+  <si>
+    <t>VPD_m1_kPa_mean</t>
+  </si>
+  <si>
+    <t>VPD_m2_kPa_mean</t>
+  </si>
+  <si>
+    <t>VPD_m3_kPa_mean</t>
+  </si>
+  <si>
+    <t>VPD_m4_kPa_mean</t>
+  </si>
+  <si>
+    <t>VPD_m5_kPa_mean</t>
+  </si>
+  <si>
+    <t>VPD_m6_kPa_mean</t>
+  </si>
+  <si>
+    <t>VPD_m7_kPa_mean</t>
+  </si>
+  <si>
+    <t>VPD_m8_kPa_mean</t>
+  </si>
+  <si>
+    <t>VPD_m9_kPa_mean</t>
+  </si>
+  <si>
+    <t>VPD_m10_kPa_mean</t>
+  </si>
+  <si>
+    <t>VPD_m11_kPa_mean</t>
+  </si>
+  <si>
+    <t>VPD_m12_kPa_mean</t>
+  </si>
+  <si>
+    <t>Mean vapor pressure deficit (kPa) in month 1</t>
+  </si>
+  <si>
+    <t>Mean vapor pressure deficit (kPa) in month 2</t>
+  </si>
+  <si>
+    <t>Mean vapor pressure deficit (kPa) in month 3</t>
+  </si>
+  <si>
+    <t>Mean vapor pressure deficit (kPa) in month 4</t>
+  </si>
+  <si>
+    <t>Mean vapor pressure deficit (kPa) in month 5</t>
+  </si>
+  <si>
+    <t>Mean vapor pressure deficit (kPa) in month 6</t>
+  </si>
+  <si>
+    <t>Mean vapor pressure deficit (kPa) in month 7</t>
+  </si>
+  <si>
+    <t>Mean vapor pressure deficit (kPa) in month 8</t>
+  </si>
+  <si>
+    <t>Mean vapor pressure deficit (kPa) in month 9</t>
+  </si>
+  <si>
+    <t>Mean vapor pressure deficit (kPa) in month 10</t>
+  </si>
+  <si>
+    <t>Mean vapor pressure deficit (kPa) in month 11</t>
+  </si>
+  <si>
+    <t>Mean vapor pressure deficit (kPa) in month 12</t>
   </si>
 </sst>
 </file>
@@ -5487,8 +5586,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="865">
+  <cellStyleXfs count="877">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -6387,7 +6498,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="865">
+  <cellStyles count="877">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -6820,6 +6931,12 @@
     <cellStyle name="Followed Hyperlink" xfId="860" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="862" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="864" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="866" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="868" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="870" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="872" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="874" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="876" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -7252,6 +7369,12 @@
     <cellStyle name="Hyperlink" xfId="859" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="861" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="863" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="865" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="867" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="869" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="871" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="873" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="875" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7581,13 +7704,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I898"/>
+  <dimension ref="A1:I910"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="8060" ySplit="860" activePane="bottomRight"/>
       <selection activeCell="C939" sqref="C939"/>
       <selection pane="topRight" activeCell="G1" sqref="G1:G1048576"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A819" sqref="A819:XFD830"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
@@ -20013,6 +20136,9 @@
       <c r="G511" s="13">
         <v>1</v>
       </c>
+      <c r="H511" s="12" t="s">
+        <v>1797</v>
+      </c>
       <c r="I511" s="12"/>
     </row>
     <row r="512" spans="1:9" s="14" customFormat="1">
@@ -20037,6 +20163,9 @@
       <c r="G512" s="13">
         <v>1</v>
       </c>
+      <c r="H512" s="12" t="s">
+        <v>1798</v>
+      </c>
       <c r="I512" s="12"/>
     </row>
     <row r="513" spans="1:9" s="14" customFormat="1">
@@ -20061,6 +20190,9 @@
       <c r="G513" s="13">
         <v>1</v>
       </c>
+      <c r="H513" s="12" t="s">
+        <v>1799</v>
+      </c>
       <c r="I513" s="12"/>
     </row>
     <row r="514" spans="1:9" s="14" customFormat="1">
@@ -20085,6 +20217,9 @@
       <c r="G514" s="13">
         <v>1</v>
       </c>
+      <c r="H514" s="1" t="s">
+        <v>1800</v>
+      </c>
       <c r="I514" s="12"/>
     </row>
     <row r="515" spans="1:9" s="14" customFormat="1">
@@ -20107,6 +20242,9 @@
       <c r="G515" s="13">
         <v>0</v>
       </c>
+      <c r="H515" s="12" t="s">
+        <v>1804</v>
+      </c>
       <c r="I515" s="12"/>
     </row>
     <row r="516" spans="1:9" s="14" customFormat="1">
@@ -20131,6 +20269,9 @@
       <c r="G516" s="13">
         <v>0</v>
       </c>
+      <c r="H516" s="12" t="s">
+        <v>1801</v>
+      </c>
       <c r="I516" s="12"/>
     </row>
     <row r="517" spans="1:9" s="14" customFormat="1">
@@ -20155,6 +20296,9 @@
       <c r="G517" s="13">
         <v>0</v>
       </c>
+      <c r="H517" s="12" t="s">
+        <v>1802</v>
+      </c>
       <c r="I517" s="12"/>
     </row>
     <row r="518" spans="1:9" s="14" customFormat="1">
@@ -20179,6 +20323,9 @@
       <c r="G518" s="13">
         <v>0</v>
       </c>
+      <c r="H518" s="1" t="s">
+        <v>1803</v>
+      </c>
       <c r="I518" s="12"/>
     </row>
     <row r="519" spans="1:9" s="14" customFormat="1">
@@ -27690,17 +27837,17 @@
         <v>1477</v>
       </c>
       <c r="D819" s="1" t="s">
-        <v>1639</v>
+        <v>1805</v>
       </c>
       <c r="E819" s="1"/>
       <c r="F819" s="1" t="s">
-        <v>527</v>
+        <v>1806</v>
       </c>
       <c r="G819" s="7">
         <v>1</v>
       </c>
       <c r="H819" s="1" t="s">
-        <v>817</v>
+        <v>1818</v>
       </c>
       <c r="I819" s="1"/>
     </row>
@@ -27715,17 +27862,17 @@
         <v>1477</v>
       </c>
       <c r="D820" s="1" t="s">
-        <v>1639</v>
+        <v>1805</v>
       </c>
       <c r="E820" s="1"/>
       <c r="F820" s="1" t="s">
-        <v>528</v>
+        <v>1807</v>
       </c>
       <c r="G820" s="7">
         <v>1</v>
       </c>
       <c r="H820" s="1" t="s">
-        <v>818</v>
+        <v>1819</v>
       </c>
       <c r="I820" s="1"/>
     </row>
@@ -27740,17 +27887,17 @@
         <v>1477</v>
       </c>
       <c r="D821" s="1" t="s">
-        <v>1639</v>
+        <v>1805</v>
       </c>
       <c r="E821" s="1"/>
       <c r="F821" s="1" t="s">
-        <v>529</v>
+        <v>1808</v>
       </c>
       <c r="G821" s="7">
         <v>1</v>
       </c>
       <c r="H821" s="1" t="s">
-        <v>819</v>
+        <v>1820</v>
       </c>
       <c r="I821" s="1"/>
     </row>
@@ -27765,17 +27912,17 @@
         <v>1477</v>
       </c>
       <c r="D822" s="1" t="s">
-        <v>1639</v>
+        <v>1805</v>
       </c>
       <c r="E822" s="1"/>
       <c r="F822" s="1" t="s">
-        <v>530</v>
+        <v>1809</v>
       </c>
       <c r="G822" s="7">
         <v>1</v>
       </c>
       <c r="H822" s="1" t="s">
-        <v>820</v>
+        <v>1821</v>
       </c>
       <c r="I822" s="1"/>
     </row>
@@ -27790,17 +27937,17 @@
         <v>1477</v>
       </c>
       <c r="D823" s="1" t="s">
-        <v>1639</v>
+        <v>1805</v>
       </c>
       <c r="E823" s="1"/>
       <c r="F823" s="1" t="s">
-        <v>531</v>
+        <v>1810</v>
       </c>
       <c r="G823" s="7">
         <v>1</v>
       </c>
       <c r="H823" s="1" t="s">
-        <v>821</v>
+        <v>1822</v>
       </c>
       <c r="I823" s="1"/>
     </row>
@@ -27815,17 +27962,17 @@
         <v>1477</v>
       </c>
       <c r="D824" s="1" t="s">
-        <v>1639</v>
+        <v>1805</v>
       </c>
       <c r="E824" s="1"/>
       <c r="F824" s="1" t="s">
-        <v>532</v>
+        <v>1811</v>
       </c>
       <c r="G824" s="7">
         <v>1</v>
       </c>
       <c r="H824" s="1" t="s">
-        <v>822</v>
+        <v>1823</v>
       </c>
       <c r="I824" s="1"/>
     </row>
@@ -27840,17 +27987,17 @@
         <v>1477</v>
       </c>
       <c r="D825" s="1" t="s">
-        <v>1639</v>
+        <v>1805</v>
       </c>
       <c r="E825" s="1"/>
       <c r="F825" s="1" t="s">
-        <v>533</v>
+        <v>1812</v>
       </c>
       <c r="G825" s="7">
         <v>1</v>
       </c>
       <c r="H825" s="1" t="s">
-        <v>823</v>
+        <v>1824</v>
       </c>
       <c r="I825" s="1"/>
     </row>
@@ -27865,17 +28012,17 @@
         <v>1477</v>
       </c>
       <c r="D826" s="1" t="s">
-        <v>1639</v>
+        <v>1805</v>
       </c>
       <c r="E826" s="1"/>
       <c r="F826" s="1" t="s">
-        <v>534</v>
+        <v>1813</v>
       </c>
       <c r="G826" s="7">
         <v>1</v>
       </c>
       <c r="H826" s="1" t="s">
-        <v>824</v>
+        <v>1825</v>
       </c>
       <c r="I826" s="1"/>
     </row>
@@ -27890,17 +28037,17 @@
         <v>1477</v>
       </c>
       <c r="D827" s="1" t="s">
-        <v>1639</v>
+        <v>1805</v>
       </c>
       <c r="E827" s="1"/>
       <c r="F827" s="1" t="s">
-        <v>535</v>
+        <v>1814</v>
       </c>
       <c r="G827" s="7">
         <v>1</v>
       </c>
       <c r="H827" s="1" t="s">
-        <v>825</v>
+        <v>1826</v>
       </c>
       <c r="I827" s="1"/>
     </row>
@@ -27915,17 +28062,17 @@
         <v>1477</v>
       </c>
       <c r="D828" s="1" t="s">
-        <v>1639</v>
+        <v>1805</v>
       </c>
       <c r="E828" s="1"/>
       <c r="F828" s="1" t="s">
-        <v>536</v>
+        <v>1815</v>
       </c>
       <c r="G828" s="7">
         <v>1</v>
       </c>
       <c r="H828" s="1" t="s">
-        <v>826</v>
+        <v>1827</v>
       </c>
       <c r="I828" s="1"/>
     </row>
@@ -27940,17 +28087,17 @@
         <v>1477</v>
       </c>
       <c r="D829" s="1" t="s">
-        <v>1639</v>
+        <v>1805</v>
       </c>
       <c r="E829" s="1"/>
       <c r="F829" s="1" t="s">
-        <v>537</v>
+        <v>1816</v>
       </c>
       <c r="G829" s="7">
         <v>1</v>
       </c>
       <c r="H829" s="1" t="s">
-        <v>827</v>
+        <v>1828</v>
       </c>
       <c r="I829" s="1"/>
     </row>
@@ -27965,17 +28112,17 @@
         <v>1477</v>
       </c>
       <c r="D830" s="1" t="s">
-        <v>1639</v>
+        <v>1805</v>
       </c>
       <c r="E830" s="1"/>
       <c r="F830" s="1" t="s">
-        <v>538</v>
+        <v>1817</v>
       </c>
       <c r="G830" s="7">
         <v>1</v>
       </c>
       <c r="H830" s="1" t="s">
-        <v>828</v>
+        <v>1829</v>
       </c>
       <c r="I830" s="1"/>
     </row>
@@ -27994,13 +28141,13 @@
       </c>
       <c r="E831" s="1"/>
       <c r="F831" s="1" t="s">
-        <v>539</v>
+        <v>527</v>
       </c>
       <c r="G831" s="7">
         <v>1</v>
       </c>
       <c r="H831" s="1" t="s">
-        <v>829</v>
+        <v>817</v>
       </c>
       <c r="I831" s="1"/>
     </row>
@@ -28019,13 +28166,13 @@
       </c>
       <c r="E832" s="1"/>
       <c r="F832" s="1" t="s">
-        <v>540</v>
+        <v>528</v>
       </c>
       <c r="G832" s="7">
         <v>1</v>
       </c>
       <c r="H832" s="1" t="s">
-        <v>830</v>
+        <v>818</v>
       </c>
       <c r="I832" s="1"/>
     </row>
@@ -28044,13 +28191,13 @@
       </c>
       <c r="E833" s="1"/>
       <c r="F833" s="1" t="s">
-        <v>541</v>
+        <v>529</v>
       </c>
       <c r="G833" s="7">
         <v>1</v>
       </c>
       <c r="H833" s="1" t="s">
-        <v>831</v>
+        <v>819</v>
       </c>
       <c r="I833" s="1"/>
     </row>
@@ -28069,13 +28216,13 @@
       </c>
       <c r="E834" s="1"/>
       <c r="F834" s="1" t="s">
-        <v>542</v>
+        <v>530</v>
       </c>
       <c r="G834" s="7">
         <v>1</v>
       </c>
       <c r="H834" s="1" t="s">
-        <v>832</v>
+        <v>820</v>
       </c>
       <c r="I834" s="1"/>
     </row>
@@ -28094,13 +28241,13 @@
       </c>
       <c r="E835" s="1"/>
       <c r="F835" s="1" t="s">
-        <v>543</v>
+        <v>531</v>
       </c>
       <c r="G835" s="7">
         <v>1</v>
       </c>
       <c r="H835" s="1" t="s">
-        <v>833</v>
+        <v>821</v>
       </c>
       <c r="I835" s="1"/>
     </row>
@@ -28119,13 +28266,13 @@
       </c>
       <c r="E836" s="1"/>
       <c r="F836" s="1" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
       <c r="G836" s="7">
         <v>1</v>
       </c>
       <c r="H836" s="1" t="s">
-        <v>834</v>
+        <v>822</v>
       </c>
       <c r="I836" s="1"/>
     </row>
@@ -28144,13 +28291,13 @@
       </c>
       <c r="E837" s="1"/>
       <c r="F837" s="1" t="s">
-        <v>545</v>
+        <v>533</v>
       </c>
       <c r="G837" s="7">
         <v>1</v>
       </c>
       <c r="H837" s="1" t="s">
-        <v>835</v>
+        <v>823</v>
       </c>
       <c r="I837" s="1"/>
     </row>
@@ -28169,13 +28316,13 @@
       </c>
       <c r="E838" s="1"/>
       <c r="F838" s="1" t="s">
-        <v>546</v>
+        <v>534</v>
       </c>
       <c r="G838" s="7">
         <v>1</v>
       </c>
       <c r="H838" s="1" t="s">
-        <v>836</v>
+        <v>824</v>
       </c>
       <c r="I838" s="1"/>
     </row>
@@ -28194,13 +28341,13 @@
       </c>
       <c r="E839" s="1"/>
       <c r="F839" s="1" t="s">
-        <v>547</v>
+        <v>535</v>
       </c>
       <c r="G839" s="7">
         <v>1</v>
       </c>
       <c r="H839" s="1" t="s">
-        <v>837</v>
+        <v>825</v>
       </c>
       <c r="I839" s="1"/>
     </row>
@@ -28219,13 +28366,13 @@
       </c>
       <c r="E840" s="1"/>
       <c r="F840" s="1" t="s">
-        <v>548</v>
+        <v>536</v>
       </c>
       <c r="G840" s="7">
         <v>1</v>
       </c>
       <c r="H840" s="1" t="s">
-        <v>838</v>
+        <v>826</v>
       </c>
       <c r="I840" s="1"/>
     </row>
@@ -28244,13 +28391,13 @@
       </c>
       <c r="E841" s="1"/>
       <c r="F841" s="1" t="s">
-        <v>549</v>
+        <v>537</v>
       </c>
       <c r="G841" s="7">
         <v>1</v>
       </c>
       <c r="H841" s="1" t="s">
-        <v>839</v>
+        <v>827</v>
       </c>
       <c r="I841" s="1"/>
     </row>
@@ -28269,13 +28416,13 @@
       </c>
       <c r="E842" s="1"/>
       <c r="F842" s="1" t="s">
-        <v>550</v>
+        <v>538</v>
       </c>
       <c r="G842" s="7">
         <v>1</v>
       </c>
       <c r="H842" s="1" t="s">
-        <v>840</v>
+        <v>828</v>
       </c>
       <c r="I842" s="1"/>
     </row>
@@ -28290,17 +28437,17 @@
         <v>1477</v>
       </c>
       <c r="D843" s="1" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="E843" s="1"/>
       <c r="F843" s="1" t="s">
-        <v>551</v>
+        <v>539</v>
       </c>
       <c r="G843" s="7">
         <v>1</v>
       </c>
       <c r="H843" s="1" t="s">
-        <v>841</v>
+        <v>829</v>
       </c>
       <c r="I843" s="1"/>
     </row>
@@ -28315,17 +28462,17 @@
         <v>1477</v>
       </c>
       <c r="D844" s="1" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="E844" s="1"/>
       <c r="F844" s="1" t="s">
-        <v>552</v>
+        <v>540</v>
       </c>
       <c r="G844" s="7">
         <v>1</v>
       </c>
       <c r="H844" s="1" t="s">
-        <v>842</v>
+        <v>830</v>
       </c>
       <c r="I844" s="1"/>
     </row>
@@ -28340,17 +28487,17 @@
         <v>1477</v>
       </c>
       <c r="D845" s="1" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="E845" s="1"/>
       <c r="F845" s="1" t="s">
-        <v>553</v>
+        <v>541</v>
       </c>
       <c r="G845" s="7">
         <v>1</v>
       </c>
       <c r="H845" s="1" t="s">
-        <v>843</v>
+        <v>831</v>
       </c>
       <c r="I845" s="1"/>
     </row>
@@ -28365,17 +28512,17 @@
         <v>1477</v>
       </c>
       <c r="D846" s="1" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="E846" s="1"/>
       <c r="F846" s="1" t="s">
-        <v>554</v>
+        <v>542</v>
       </c>
       <c r="G846" s="7">
         <v>1</v>
       </c>
       <c r="H846" s="1" t="s">
-        <v>844</v>
+        <v>832</v>
       </c>
       <c r="I846" s="1"/>
     </row>
@@ -28390,17 +28537,17 @@
         <v>1477</v>
       </c>
       <c r="D847" s="1" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="E847" s="1"/>
       <c r="F847" s="1" t="s">
-        <v>555</v>
+        <v>543</v>
       </c>
       <c r="G847" s="7">
         <v>1</v>
       </c>
       <c r="H847" s="1" t="s">
-        <v>845</v>
+        <v>833</v>
       </c>
       <c r="I847" s="1"/>
     </row>
@@ -28415,17 +28562,17 @@
         <v>1477</v>
       </c>
       <c r="D848" s="1" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="E848" s="1"/>
       <c r="F848" s="1" t="s">
-        <v>556</v>
+        <v>544</v>
       </c>
       <c r="G848" s="7">
         <v>1</v>
       </c>
       <c r="H848" s="1" t="s">
-        <v>846</v>
+        <v>834</v>
       </c>
       <c r="I848" s="1"/>
     </row>
@@ -28440,17 +28587,17 @@
         <v>1477</v>
       </c>
       <c r="D849" s="1" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="E849" s="1"/>
       <c r="F849" s="1" t="s">
-        <v>557</v>
+        <v>545</v>
       </c>
       <c r="G849" s="7">
         <v>1</v>
       </c>
       <c r="H849" s="1" t="s">
-        <v>847</v>
+        <v>835</v>
       </c>
       <c r="I849" s="1"/>
     </row>
@@ -28465,17 +28612,17 @@
         <v>1477</v>
       </c>
       <c r="D850" s="1" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="E850" s="1"/>
       <c r="F850" s="1" t="s">
-        <v>558</v>
+        <v>546</v>
       </c>
       <c r="G850" s="7">
         <v>1</v>
       </c>
       <c r="H850" s="1" t="s">
-        <v>848</v>
+        <v>836</v>
       </c>
       <c r="I850" s="1"/>
     </row>
@@ -28490,17 +28637,17 @@
         <v>1477</v>
       </c>
       <c r="D851" s="1" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="E851" s="1"/>
       <c r="F851" s="1" t="s">
-        <v>559</v>
+        <v>547</v>
       </c>
       <c r="G851" s="7">
         <v>1</v>
       </c>
       <c r="H851" s="1" t="s">
-        <v>849</v>
+        <v>837</v>
       </c>
       <c r="I851" s="1"/>
     </row>
@@ -28515,17 +28662,17 @@
         <v>1477</v>
       </c>
       <c r="D852" s="1" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="E852" s="1"/>
       <c r="F852" s="1" t="s">
-        <v>560</v>
+        <v>548</v>
       </c>
       <c r="G852" s="7">
         <v>1</v>
       </c>
       <c r="H852" s="1" t="s">
-        <v>850</v>
+        <v>838</v>
       </c>
       <c r="I852" s="1"/>
     </row>
@@ -28540,17 +28687,17 @@
         <v>1477</v>
       </c>
       <c r="D853" s="1" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="E853" s="1"/>
       <c r="F853" s="1" t="s">
-        <v>561</v>
+        <v>549</v>
       </c>
       <c r="G853" s="7">
         <v>1</v>
       </c>
       <c r="H853" s="1" t="s">
-        <v>851</v>
+        <v>839</v>
       </c>
       <c r="I853" s="1"/>
     </row>
@@ -28565,17 +28712,17 @@
         <v>1477</v>
       </c>
       <c r="D854" s="1" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="E854" s="1"/>
       <c r="F854" s="1" t="s">
-        <v>562</v>
+        <v>550</v>
       </c>
       <c r="G854" s="7">
         <v>1</v>
       </c>
       <c r="H854" s="1" t="s">
-        <v>852</v>
+        <v>840</v>
       </c>
       <c r="I854" s="1"/>
     </row>
@@ -28594,13 +28741,13 @@
       </c>
       <c r="E855" s="1"/>
       <c r="F855" s="1" t="s">
-        <v>563</v>
+        <v>551</v>
       </c>
       <c r="G855" s="7">
         <v>1</v>
       </c>
       <c r="H855" s="1" t="s">
-        <v>853</v>
+        <v>841</v>
       </c>
       <c r="I855" s="1"/>
     </row>
@@ -28619,13 +28766,13 @@
       </c>
       <c r="E856" s="1"/>
       <c r="F856" s="1" t="s">
-        <v>564</v>
+        <v>552</v>
       </c>
       <c r="G856" s="7">
         <v>1</v>
       </c>
       <c r="H856" s="1" t="s">
-        <v>854</v>
+        <v>842</v>
       </c>
       <c r="I856" s="1"/>
     </row>
@@ -28644,13 +28791,13 @@
       </c>
       <c r="E857" s="1"/>
       <c r="F857" s="1" t="s">
-        <v>565</v>
+        <v>553</v>
       </c>
       <c r="G857" s="7">
         <v>1</v>
       </c>
       <c r="H857" s="1" t="s">
-        <v>855</v>
+        <v>843</v>
       </c>
       <c r="I857" s="1"/>
     </row>
@@ -28669,13 +28816,13 @@
       </c>
       <c r="E858" s="1"/>
       <c r="F858" s="1" t="s">
-        <v>566</v>
+        <v>554</v>
       </c>
       <c r="G858" s="7">
         <v>1</v>
       </c>
       <c r="H858" s="1" t="s">
-        <v>856</v>
+        <v>844</v>
       </c>
       <c r="I858" s="1"/>
     </row>
@@ -28694,13 +28841,13 @@
       </c>
       <c r="E859" s="1"/>
       <c r="F859" s="1" t="s">
-        <v>567</v>
+        <v>555</v>
       </c>
       <c r="G859" s="7">
         <v>1</v>
       </c>
       <c r="H859" s="1" t="s">
-        <v>857</v>
+        <v>845</v>
       </c>
       <c r="I859" s="1"/>
     </row>
@@ -28719,13 +28866,13 @@
       </c>
       <c r="E860" s="1"/>
       <c r="F860" s="1" t="s">
-        <v>568</v>
+        <v>556</v>
       </c>
       <c r="G860" s="7">
         <v>1</v>
       </c>
       <c r="H860" s="1" t="s">
-        <v>858</v>
+        <v>846</v>
       </c>
       <c r="I860" s="1"/>
     </row>
@@ -28744,13 +28891,13 @@
       </c>
       <c r="E861" s="1"/>
       <c r="F861" s="1" t="s">
-        <v>569</v>
+        <v>557</v>
       </c>
       <c r="G861" s="7">
         <v>1</v>
       </c>
       <c r="H861" s="1" t="s">
-        <v>859</v>
+        <v>847</v>
       </c>
       <c r="I861" s="1"/>
     </row>
@@ -28769,13 +28916,13 @@
       </c>
       <c r="E862" s="1"/>
       <c r="F862" s="1" t="s">
-        <v>570</v>
+        <v>558</v>
       </c>
       <c r="G862" s="7">
         <v>1</v>
       </c>
       <c r="H862" s="1" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="I862" s="1"/>
     </row>
@@ -28794,13 +28941,13 @@
       </c>
       <c r="E863" s="1"/>
       <c r="F863" s="1" t="s">
-        <v>571</v>
+        <v>559</v>
       </c>
       <c r="G863" s="7">
         <v>1</v>
       </c>
       <c r="H863" s="1" t="s">
-        <v>861</v>
+        <v>849</v>
       </c>
       <c r="I863" s="1"/>
     </row>
@@ -28819,13 +28966,13 @@
       </c>
       <c r="E864" s="1"/>
       <c r="F864" s="1" t="s">
-        <v>572</v>
+        <v>560</v>
       </c>
       <c r="G864" s="7">
         <v>1</v>
       </c>
       <c r="H864" s="1" t="s">
-        <v>862</v>
+        <v>850</v>
       </c>
       <c r="I864" s="1"/>
     </row>
@@ -28844,13 +28991,13 @@
       </c>
       <c r="E865" s="1"/>
       <c r="F865" s="1" t="s">
-        <v>573</v>
+        <v>561</v>
       </c>
       <c r="G865" s="7">
         <v>1</v>
       </c>
       <c r="H865" s="1" t="s">
-        <v>863</v>
+        <v>851</v>
       </c>
       <c r="I865" s="1"/>
     </row>
@@ -28869,13 +29016,13 @@
       </c>
       <c r="E866" s="1"/>
       <c r="F866" s="1" t="s">
-        <v>574</v>
+        <v>562</v>
       </c>
       <c r="G866" s="7">
         <v>1</v>
       </c>
       <c r="H866" s="1" t="s">
-        <v>864</v>
+        <v>852</v>
       </c>
       <c r="I866" s="1"/>
     </row>
@@ -28887,19 +29034,21 @@
         <v>898</v>
       </c>
       <c r="C867" s="1" t="s">
-        <v>1702</v>
+        <v>1477</v>
       </c>
       <c r="D867" s="1" t="s">
-        <v>1667</v>
+        <v>1640</v>
       </c>
       <c r="E867" s="1"/>
       <c r="F867" s="1" t="s">
-        <v>1668</v>
+        <v>563</v>
       </c>
       <c r="G867" s="7">
         <v>1</v>
       </c>
-      <c r="H867" s="1"/>
+      <c r="H867" s="1" t="s">
+        <v>853</v>
+      </c>
       <c r="I867" s="1"/>
     </row>
     <row r="868" spans="1:9">
@@ -28910,20 +29059,22 @@
         <v>898</v>
       </c>
       <c r="C868" s="1" t="s">
-        <v>1702</v>
-      </c>
-      <c r="D868" s="2" t="s">
-        <v>1701</v>
-      </c>
-      <c r="E868" s="2" t="s">
-        <v>1700</v>
-      </c>
-      <c r="F868" s="2" t="s">
-        <v>1669</v>
+        <v>1477</v>
+      </c>
+      <c r="D868" s="1" t="s">
+        <v>1640</v>
+      </c>
+      <c r="E868" s="1"/>
+      <c r="F868" s="1" t="s">
+        <v>564</v>
       </c>
       <c r="G868" s="7">
         <v>1</v>
       </c>
+      <c r="H868" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="I868" s="1"/>
     </row>
     <row r="869" spans="1:9">
       <c r="A869" s="1">
@@ -28933,20 +29084,22 @@
         <v>898</v>
       </c>
       <c r="C869" s="1" t="s">
-        <v>1702</v>
-      </c>
-      <c r="D869" s="2" t="s">
-        <v>1701</v>
-      </c>
-      <c r="E869" s="2" t="s">
-        <v>1700</v>
-      </c>
-      <c r="F869" s="2" t="s">
-        <v>1670</v>
+        <v>1477</v>
+      </c>
+      <c r="D869" s="1" t="s">
+        <v>1640</v>
+      </c>
+      <c r="E869" s="1"/>
+      <c r="F869" s="1" t="s">
+        <v>565</v>
       </c>
       <c r="G869" s="7">
         <v>1</v>
       </c>
+      <c r="H869" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="I869" s="1"/>
     </row>
     <row r="870" spans="1:9">
       <c r="A870" s="1">
@@ -28956,20 +29109,22 @@
         <v>898</v>
       </c>
       <c r="C870" s="1" t="s">
-        <v>1702</v>
-      </c>
-      <c r="D870" s="2" t="s">
-        <v>1701</v>
-      </c>
-      <c r="E870" s="2" t="s">
-        <v>1700</v>
-      </c>
-      <c r="F870" s="2" t="s">
-        <v>1671</v>
-      </c>
-      <c r="G870" s="8">
-        <v>0</v>
-      </c>
+        <v>1477</v>
+      </c>
+      <c r="D870" s="1" t="s">
+        <v>1640</v>
+      </c>
+      <c r="E870" s="1"/>
+      <c r="F870" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="G870" s="7">
+        <v>1</v>
+      </c>
+      <c r="H870" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="I870" s="1"/>
     </row>
     <row r="871" spans="1:9">
       <c r="A871" s="1">
@@ -28979,20 +29134,22 @@
         <v>898</v>
       </c>
       <c r="C871" s="1" t="s">
-        <v>1702</v>
-      </c>
-      <c r="D871" s="2" t="s">
-        <v>1701</v>
-      </c>
-      <c r="E871" s="2" t="s">
-        <v>1700</v>
-      </c>
-      <c r="F871" s="2" t="s">
-        <v>1672</v>
-      </c>
-      <c r="G871" s="8">
-        <v>0</v>
-      </c>
+        <v>1477</v>
+      </c>
+      <c r="D871" s="1" t="s">
+        <v>1640</v>
+      </c>
+      <c r="E871" s="1"/>
+      <c r="F871" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="G871" s="7">
+        <v>1</v>
+      </c>
+      <c r="H871" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="I871" s="1"/>
     </row>
     <row r="872" spans="1:9">
       <c r="A872" s="1">
@@ -29002,20 +29159,22 @@
         <v>898</v>
       </c>
       <c r="C872" s="1" t="s">
-        <v>1702</v>
-      </c>
-      <c r="D872" s="2" t="s">
-        <v>1701</v>
-      </c>
-      <c r="E872" s="2" t="s">
-        <v>1700</v>
-      </c>
-      <c r="F872" s="2" t="s">
-        <v>1673</v>
-      </c>
-      <c r="G872" s="8">
-        <v>0</v>
-      </c>
+        <v>1477</v>
+      </c>
+      <c r="D872" s="1" t="s">
+        <v>1640</v>
+      </c>
+      <c r="E872" s="1"/>
+      <c r="F872" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="G872" s="7">
+        <v>1</v>
+      </c>
+      <c r="H872" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="I872" s="1"/>
     </row>
     <row r="873" spans="1:9">
       <c r="A873" s="1">
@@ -29025,20 +29184,22 @@
         <v>898</v>
       </c>
       <c r="C873" s="1" t="s">
-        <v>1702</v>
-      </c>
-      <c r="D873" s="2" t="s">
-        <v>1701</v>
-      </c>
-      <c r="E873" s="2" t="s">
-        <v>1700</v>
-      </c>
-      <c r="F873" s="2" t="s">
-        <v>1674</v>
-      </c>
-      <c r="G873" s="8">
-        <v>0</v>
-      </c>
+        <v>1477</v>
+      </c>
+      <c r="D873" s="1" t="s">
+        <v>1640</v>
+      </c>
+      <c r="E873" s="1"/>
+      <c r="F873" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="G873" s="7">
+        <v>1</v>
+      </c>
+      <c r="H873" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="I873" s="1"/>
     </row>
     <row r="874" spans="1:9">
       <c r="A874" s="1">
@@ -29048,20 +29209,22 @@
         <v>898</v>
       </c>
       <c r="C874" s="1" t="s">
-        <v>1702</v>
-      </c>
-      <c r="D874" s="2" t="s">
-        <v>1701</v>
-      </c>
-      <c r="E874" s="2" t="s">
-        <v>1700</v>
-      </c>
-      <c r="F874" s="2" t="s">
-        <v>1675</v>
-      </c>
-      <c r="G874" s="8">
-        <v>0</v>
-      </c>
+        <v>1477</v>
+      </c>
+      <c r="D874" s="1" t="s">
+        <v>1640</v>
+      </c>
+      <c r="E874" s="1"/>
+      <c r="F874" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="G874" s="7">
+        <v>1</v>
+      </c>
+      <c r="H874" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="I874" s="1"/>
     </row>
     <row r="875" spans="1:9">
       <c r="A875" s="1">
@@ -29071,20 +29234,22 @@
         <v>898</v>
       </c>
       <c r="C875" s="1" t="s">
-        <v>1702</v>
-      </c>
-      <c r="D875" s="2" t="s">
-        <v>1701</v>
-      </c>
-      <c r="E875" s="2" t="s">
-        <v>1700</v>
-      </c>
-      <c r="F875" s="2" t="s">
-        <v>1676</v>
-      </c>
-      <c r="G875" s="8">
-        <v>0</v>
-      </c>
+        <v>1477</v>
+      </c>
+      <c r="D875" s="1" t="s">
+        <v>1640</v>
+      </c>
+      <c r="E875" s="1"/>
+      <c r="F875" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="G875" s="7">
+        <v>1</v>
+      </c>
+      <c r="H875" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="I875" s="1"/>
     </row>
     <row r="876" spans="1:9">
       <c r="A876" s="1">
@@ -29094,20 +29259,22 @@
         <v>898</v>
       </c>
       <c r="C876" s="1" t="s">
-        <v>1702</v>
-      </c>
-      <c r="D876" s="2" t="s">
-        <v>1701</v>
-      </c>
-      <c r="E876" s="2" t="s">
-        <v>1700</v>
-      </c>
-      <c r="F876" s="2" t="s">
-        <v>1677</v>
-      </c>
-      <c r="G876" s="8">
-        <v>1</v>
-      </c>
+        <v>1477</v>
+      </c>
+      <c r="D876" s="1" t="s">
+        <v>1640</v>
+      </c>
+      <c r="E876" s="1"/>
+      <c r="F876" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="G876" s="7">
+        <v>1</v>
+      </c>
+      <c r="H876" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="I876" s="1"/>
     </row>
     <row r="877" spans="1:9">
       <c r="A877" s="1">
@@ -29117,20 +29284,22 @@
         <v>898</v>
       </c>
       <c r="C877" s="1" t="s">
-        <v>1702</v>
-      </c>
-      <c r="D877" s="2" t="s">
-        <v>1701</v>
-      </c>
-      <c r="E877" s="2" t="s">
-        <v>1700</v>
-      </c>
-      <c r="F877" s="2" t="s">
-        <v>1678</v>
-      </c>
-      <c r="G877" s="8">
-        <v>1</v>
-      </c>
+        <v>1477</v>
+      </c>
+      <c r="D877" s="1" t="s">
+        <v>1640</v>
+      </c>
+      <c r="E877" s="1"/>
+      <c r="F877" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="G877" s="7">
+        <v>1</v>
+      </c>
+      <c r="H877" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="I877" s="1"/>
     </row>
     <row r="878" spans="1:9">
       <c r="A878" s="1">
@@ -29140,20 +29309,22 @@
         <v>898</v>
       </c>
       <c r="C878" s="1" t="s">
-        <v>1702</v>
-      </c>
-      <c r="D878" s="2" t="s">
-        <v>1701</v>
-      </c>
-      <c r="E878" s="2" t="s">
-        <v>1700</v>
-      </c>
-      <c r="F878" s="2" t="s">
-        <v>1679</v>
-      </c>
-      <c r="G878" s="8">
-        <v>0</v>
-      </c>
+        <v>1477</v>
+      </c>
+      <c r="D878" s="1" t="s">
+        <v>1640</v>
+      </c>
+      <c r="E878" s="1"/>
+      <c r="F878" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="G878" s="7">
+        <v>1</v>
+      </c>
+      <c r="H878" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="I878" s="1"/>
     </row>
     <row r="879" spans="1:9">
       <c r="A879" s="1">
@@ -29165,18 +29336,18 @@
       <c r="C879" s="1" t="s">
         <v>1702</v>
       </c>
-      <c r="D879" s="2" t="s">
-        <v>1701</v>
-      </c>
-      <c r="E879" s="2" t="s">
-        <v>1700</v>
-      </c>
-      <c r="F879" s="2" t="s">
-        <v>1680</v>
-      </c>
-      <c r="G879" s="8">
-        <v>0</v>
-      </c>
+      <c r="D879" s="1" t="s">
+        <v>1667</v>
+      </c>
+      <c r="E879" s="1"/>
+      <c r="F879" s="1" t="s">
+        <v>1668</v>
+      </c>
+      <c r="G879" s="7">
+        <v>1</v>
+      </c>
+      <c r="H879" s="1"/>
+      <c r="I879" s="1"/>
     </row>
     <row r="880" spans="1:9">
       <c r="A880" s="1">
@@ -29195,10 +29366,10 @@
         <v>1700</v>
       </c>
       <c r="F880" s="2" t="s">
-        <v>1681</v>
-      </c>
-      <c r="G880" s="8">
-        <v>0</v>
+        <v>1669</v>
+      </c>
+      <c r="G880" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="881" spans="1:7">
@@ -29218,10 +29389,10 @@
         <v>1700</v>
       </c>
       <c r="F881" s="2" t="s">
-        <v>1682</v>
-      </c>
-      <c r="G881" s="8">
-        <v>0</v>
+        <v>1670</v>
+      </c>
+      <c r="G881" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="882" spans="1:7">
@@ -29241,7 +29412,7 @@
         <v>1700</v>
       </c>
       <c r="F882" s="2" t="s">
-        <v>1683</v>
+        <v>1671</v>
       </c>
       <c r="G882" s="8">
         <v>0</v>
@@ -29264,7 +29435,7 @@
         <v>1700</v>
       </c>
       <c r="F883" s="2" t="s">
-        <v>1684</v>
+        <v>1672</v>
       </c>
       <c r="G883" s="8">
         <v>0</v>
@@ -29287,10 +29458,10 @@
         <v>1700</v>
       </c>
       <c r="F884" s="2" t="s">
-        <v>1685</v>
-      </c>
-      <c r="G884" s="10">
-        <v>1</v>
+        <v>1673</v>
+      </c>
+      <c r="G884" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="885" spans="1:7">
@@ -29310,10 +29481,10 @@
         <v>1700</v>
       </c>
       <c r="F885" s="2" t="s">
-        <v>1686</v>
-      </c>
-      <c r="G885" s="10">
-        <v>1</v>
+        <v>1674</v>
+      </c>
+      <c r="G885" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="886" spans="1:7">
@@ -29333,10 +29504,10 @@
         <v>1700</v>
       </c>
       <c r="F886" s="2" t="s">
-        <v>1687</v>
-      </c>
-      <c r="G886" s="10">
-        <v>1</v>
+        <v>1675</v>
+      </c>
+      <c r="G886" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="887" spans="1:7">
@@ -29356,10 +29527,10 @@
         <v>1700</v>
       </c>
       <c r="F887" s="2" t="s">
-        <v>1688</v>
-      </c>
-      <c r="G887" s="10">
-        <v>1</v>
+        <v>1676</v>
+      </c>
+      <c r="G887" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="888" spans="1:7">
@@ -29379,9 +29550,9 @@
         <v>1700</v>
       </c>
       <c r="F888" s="2" t="s">
-        <v>1689</v>
-      </c>
-      <c r="G888" s="10">
+        <v>1677</v>
+      </c>
+      <c r="G888" s="8">
         <v>1</v>
       </c>
     </row>
@@ -29402,9 +29573,9 @@
         <v>1700</v>
       </c>
       <c r="F889" s="2" t="s">
-        <v>1690</v>
-      </c>
-      <c r="G889" s="10">
+        <v>1678</v>
+      </c>
+      <c r="G889" s="8">
         <v>1</v>
       </c>
     </row>
@@ -29425,10 +29596,10 @@
         <v>1700</v>
       </c>
       <c r="F890" s="2" t="s">
-        <v>1691</v>
-      </c>
-      <c r="G890" s="10">
-        <v>1</v>
+        <v>1679</v>
+      </c>
+      <c r="G890" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="891" spans="1:7">
@@ -29448,10 +29619,10 @@
         <v>1700</v>
       </c>
       <c r="F891" s="2" t="s">
-        <v>1692</v>
-      </c>
-      <c r="G891" s="10">
-        <v>1</v>
+        <v>1680</v>
+      </c>
+      <c r="G891" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="892" spans="1:7">
@@ -29471,10 +29642,10 @@
         <v>1700</v>
       </c>
       <c r="F892" s="2" t="s">
-        <v>1693</v>
-      </c>
-      <c r="G892" s="10">
-        <v>1</v>
+        <v>1681</v>
+      </c>
+      <c r="G892" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="893" spans="1:7">
@@ -29494,10 +29665,10 @@
         <v>1700</v>
       </c>
       <c r="F893" s="2" t="s">
-        <v>1694</v>
-      </c>
-      <c r="G893" s="10">
-        <v>1</v>
+        <v>1682</v>
+      </c>
+      <c r="G893" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="894" spans="1:7">
@@ -29517,10 +29688,10 @@
         <v>1700</v>
       </c>
       <c r="F894" s="2" t="s">
-        <v>1695</v>
-      </c>
-      <c r="G894" s="10">
-        <v>1</v>
+        <v>1683</v>
+      </c>
+      <c r="G894" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="895" spans="1:7">
@@ -29540,10 +29711,10 @@
         <v>1700</v>
       </c>
       <c r="F895" s="2" t="s">
-        <v>1696</v>
-      </c>
-      <c r="G895" s="10">
-        <v>1</v>
+        <v>1684</v>
+      </c>
+      <c r="G895" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="896" spans="1:7">
@@ -29563,7 +29734,7 @@
         <v>1700</v>
       </c>
       <c r="F896" s="2" t="s">
-        <v>1697</v>
+        <v>1685</v>
       </c>
       <c r="G896" s="10">
         <v>1</v>
@@ -29586,7 +29757,7 @@
         <v>1700</v>
       </c>
       <c r="F897" s="2" t="s">
-        <v>1698</v>
+        <v>1686</v>
       </c>
       <c r="G897" s="10">
         <v>1</v>
@@ -29609,9 +29780,285 @@
         <v>1700</v>
       </c>
       <c r="F898" s="2" t="s">
+        <v>1687</v>
+      </c>
+      <c r="G898" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="899" spans="1:7">
+      <c r="A899" s="1">
+        <v>898</v>
+      </c>
+      <c r="B899" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="C899" s="1" t="s">
+        <v>1702</v>
+      </c>
+      <c r="D899" s="2" t="s">
+        <v>1701</v>
+      </c>
+      <c r="E899" s="2" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F899" s="2" t="s">
+        <v>1688</v>
+      </c>
+      <c r="G899" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="900" spans="1:7">
+      <c r="A900" s="1">
+        <v>899</v>
+      </c>
+      <c r="B900" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="C900" s="1" t="s">
+        <v>1702</v>
+      </c>
+      <c r="D900" s="2" t="s">
+        <v>1701</v>
+      </c>
+      <c r="E900" s="2" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F900" s="2" t="s">
+        <v>1689</v>
+      </c>
+      <c r="G900" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="901" spans="1:7">
+      <c r="A901" s="1">
+        <v>900</v>
+      </c>
+      <c r="B901" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="C901" s="1" t="s">
+        <v>1702</v>
+      </c>
+      <c r="D901" s="2" t="s">
+        <v>1701</v>
+      </c>
+      <c r="E901" s="2" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F901" s="2" t="s">
+        <v>1690</v>
+      </c>
+      <c r="G901" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="902" spans="1:7">
+      <c r="A902" s="1">
+        <v>901</v>
+      </c>
+      <c r="B902" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="C902" s="1" t="s">
+        <v>1702</v>
+      </c>
+      <c r="D902" s="2" t="s">
+        <v>1701</v>
+      </c>
+      <c r="E902" s="2" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F902" s="2" t="s">
+        <v>1691</v>
+      </c>
+      <c r="G902" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="903" spans="1:7">
+      <c r="A903" s="1">
+        <v>902</v>
+      </c>
+      <c r="B903" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="C903" s="1" t="s">
+        <v>1702</v>
+      </c>
+      <c r="D903" s="2" t="s">
+        <v>1701</v>
+      </c>
+      <c r="E903" s="2" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F903" s="2" t="s">
+        <v>1692</v>
+      </c>
+      <c r="G903" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="904" spans="1:7">
+      <c r="A904" s="1">
+        <v>903</v>
+      </c>
+      <c r="B904" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="C904" s="1" t="s">
+        <v>1702</v>
+      </c>
+      <c r="D904" s="2" t="s">
+        <v>1701</v>
+      </c>
+      <c r="E904" s="2" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F904" s="2" t="s">
+        <v>1693</v>
+      </c>
+      <c r="G904" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="905" spans="1:7">
+      <c r="A905" s="1">
+        <v>904</v>
+      </c>
+      <c r="B905" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="C905" s="1" t="s">
+        <v>1702</v>
+      </c>
+      <c r="D905" s="2" t="s">
+        <v>1701</v>
+      </c>
+      <c r="E905" s="2" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F905" s="2" t="s">
+        <v>1694</v>
+      </c>
+      <c r="G905" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="906" spans="1:7">
+      <c r="A906" s="1">
+        <v>905</v>
+      </c>
+      <c r="B906" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="C906" s="1" t="s">
+        <v>1702</v>
+      </c>
+      <c r="D906" s="2" t="s">
+        <v>1701</v>
+      </c>
+      <c r="E906" s="2" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F906" s="2" t="s">
+        <v>1695</v>
+      </c>
+      <c r="G906" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="907" spans="1:7">
+      <c r="A907" s="1">
+        <v>906</v>
+      </c>
+      <c r="B907" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="C907" s="1" t="s">
+        <v>1702</v>
+      </c>
+      <c r="D907" s="2" t="s">
+        <v>1701</v>
+      </c>
+      <c r="E907" s="2" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F907" s="2" t="s">
+        <v>1696</v>
+      </c>
+      <c r="G907" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="908" spans="1:7">
+      <c r="A908" s="1">
+        <v>907</v>
+      </c>
+      <c r="B908" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="C908" s="1" t="s">
+        <v>1702</v>
+      </c>
+      <c r="D908" s="2" t="s">
+        <v>1701</v>
+      </c>
+      <c r="E908" s="2" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F908" s="2" t="s">
+        <v>1697</v>
+      </c>
+      <c r="G908" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="909" spans="1:7">
+      <c r="A909" s="1">
+        <v>908</v>
+      </c>
+      <c r="B909" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="C909" s="1" t="s">
+        <v>1702</v>
+      </c>
+      <c r="D909" s="2" t="s">
+        <v>1701</v>
+      </c>
+      <c r="E909" s="2" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F909" s="2" t="s">
+        <v>1698</v>
+      </c>
+      <c r="G909" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="910" spans="1:7">
+      <c r="A910" s="1">
+        <v>909</v>
+      </c>
+      <c r="B910" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="C910" s="1" t="s">
+        <v>1702</v>
+      </c>
+      <c r="D910" s="2" t="s">
+        <v>1701</v>
+      </c>
+      <c r="E910" s="2" t="s">
+        <v>1700</v>
+      </c>
+      <c r="F910" s="2" t="s">
         <v>1699</v>
       </c>
-      <c r="G898" s="10">
+      <c r="G910" s="10">
         <v>1</v>
       </c>
     </row>

</xml_diff>